<commit_message>
full work 1 table
</commit_message>
<xml_diff>
--- a/api/exp_template.xlsx
+++ b/api/exp_template.xlsx
@@ -9,17 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="900" windowWidth="25410" windowHeight="12015"/>
+    <workbookView xWindow="0" yWindow="1350" windowWidth="25410" windowHeight="12015"/>
   </bookViews>
   <sheets>
     <sheet name="Персонал по стажу" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
   <si>
     <t>Приложение 5</t>
   </si>
@@ -67,72 +67,6 @@
   </si>
   <si>
     <t>20 и более</t>
-  </si>
-  <si>
-    <t>Численность работников - всего (сумма строк 02, 06, 21, 22)</t>
-  </si>
-  <si>
-    <t>в том числе: руководящие работники - всего</t>
-  </si>
-  <si>
-    <t>из них: директор (начальник)</t>
-  </si>
-  <si>
-    <t>из них: заместители директора (начальника)</t>
-  </si>
-  <si>
-    <t>из них: руководитель филиала</t>
-  </si>
-  <si>
-    <t>в том числе: педагогические работники - всего (сумма строк 07,12-20)</t>
-  </si>
-  <si>
-    <t>в том числе: преподаватели - всего (сумма строк 8-11)</t>
-  </si>
-  <si>
-    <t>из них: общеобразовательных дисциплин</t>
-  </si>
-  <si>
-    <t>из них: общего гуманитарного и социально-экономического учебного цикла</t>
-  </si>
-  <si>
-    <t>из них: математического и общего естественнонаучного учебного цикла</t>
-  </si>
-  <si>
-    <t>из них: профессионального учебного цикла</t>
-  </si>
-  <si>
-    <t>в том числе: мастера производственного обучения</t>
-  </si>
-  <si>
-    <t>в том числе: социальные педагоги</t>
-  </si>
-  <si>
-    <t>в том числе: педагоги-психологи</t>
-  </si>
-  <si>
-    <t>в том числе: педагоги-организаторы</t>
-  </si>
-  <si>
-    <t>в том числе: преподаватели-организаторы (основ безопасности жизнедеятельности, допризывной подготовки)</t>
-  </si>
-  <si>
-    <t>в том числе: руководители физического воспитания</t>
-  </si>
-  <si>
-    <t>в том числе: методисты</t>
-  </si>
-  <si>
-    <t>в том числе: тьюторы</t>
-  </si>
-  <si>
-    <t>в том числе: прочие</t>
-  </si>
-  <si>
-    <t>в том числе: учебно-вспомогательный персонал</t>
-  </si>
-  <si>
-    <t>в том числе: обслуживающий персонал</t>
   </si>
 </sst>
 </file>
@@ -464,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R29"/>
+  <dimension ref="A1:R106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -665,14 +599,10 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
-      <c r="B8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="5">
-        <v>1</v>
-      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
@@ -680,7 +610,10 @@
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
+      <c r="K8" s="5">
+        <f>SUM(L8+M8+N8+O8+P8+Q8)</f>
+        <v>0</v>
+      </c>
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
@@ -689,14 +622,10 @@
       <c r="Q8" s="5"/>
       <c r="R8" s="5"/>
     </row>
-    <row r="9" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
-      <c r="B9" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="5">
-        <v>2</v>
-      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
@@ -704,7 +633,10 @@
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
+      <c r="K9" s="5">
+        <f t="shared" ref="K9:K72" si="0">SUM(L9+M9+N9+O9+P9+Q9)</f>
+        <v>0</v>
+      </c>
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
       <c r="N9" s="5"/>
@@ -713,14 +645,10 @@
       <c r="Q9" s="5"/>
       <c r="R9" s="5"/>
     </row>
-    <row r="10" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
-      <c r="B10" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="5">
-        <v>3</v>
-      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
@@ -728,7 +656,10 @@
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
+      <c r="K10" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
@@ -737,14 +668,10 @@
       <c r="Q10" s="5"/>
       <c r="R10" s="5"/>
     </row>
-    <row r="11" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
-      <c r="B11" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="5">
-        <v>4</v>
-      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
@@ -752,7 +679,10 @@
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
+      <c r="K11" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
       <c r="N11" s="5"/>
@@ -761,14 +691,10 @@
       <c r="Q11" s="5"/>
       <c r="R11" s="5"/>
     </row>
-    <row r="12" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
-      <c r="B12" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="5">
-        <v>5</v>
-      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
@@ -776,7 +702,10 @@
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
+      <c r="K12" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
       <c r="N12" s="5"/>
@@ -785,14 +714,10 @@
       <c r="Q12" s="5"/>
       <c r="R12" s="5"/>
     </row>
-    <row r="13" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
-      <c r="B13" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="5">
-        <v>6</v>
-      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
@@ -800,7 +725,10 @@
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
+      <c r="K13" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
       <c r="N13" s="5"/>
@@ -809,14 +737,10 @@
       <c r="Q13" s="5"/>
       <c r="R13" s="5"/>
     </row>
-    <row r="14" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
-      <c r="B14" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="5">
-        <v>7</v>
-      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
@@ -824,7 +748,10 @@
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
+      <c r="K14" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
       <c r="N14" s="5"/>
@@ -833,14 +760,10 @@
       <c r="Q14" s="5"/>
       <c r="R14" s="5"/>
     </row>
-    <row r="15" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
-      <c r="B15" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="5">
-        <v>8</v>
-      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
@@ -848,7 +771,10 @@
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
+      <c r="K15" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
       <c r="N15" s="5"/>
@@ -857,14 +783,10 @@
       <c r="Q15" s="5"/>
       <c r="R15" s="5"/>
     </row>
-    <row r="16" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
-      <c r="B16" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="5">
-        <v>9</v>
-      </c>
+      <c r="B16" s="4"/>
+      <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
@@ -872,7 +794,10 @@
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
+      <c r="K16" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="L16" s="5"/>
       <c r="M16" s="5"/>
       <c r="N16" s="5"/>
@@ -881,14 +806,10 @@
       <c r="Q16" s="5"/>
       <c r="R16" s="5"/>
     </row>
-    <row r="17" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
-      <c r="B17" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="5">
-        <v>10</v>
-      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
@@ -896,7 +817,10 @@
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
+      <c r="K17" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="L17" s="5"/>
       <c r="M17" s="5"/>
       <c r="N17" s="5"/>
@@ -905,14 +829,10 @@
       <c r="Q17" s="5"/>
       <c r="R17" s="5"/>
     </row>
-    <row r="18" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
-      <c r="B18" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="5">
-        <v>11</v>
-      </c>
+      <c r="B18" s="4"/>
+      <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
@@ -920,7 +840,10 @@
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
+      <c r="K18" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="L18" s="5"/>
       <c r="M18" s="5"/>
       <c r="N18" s="5"/>
@@ -929,14 +852,10 @@
       <c r="Q18" s="5"/>
       <c r="R18" s="5"/>
     </row>
-    <row r="19" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
-      <c r="B19" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="5">
-        <v>12</v>
-      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
@@ -944,7 +863,10 @@
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
+      <c r="K19" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="L19" s="5"/>
       <c r="M19" s="5"/>
       <c r="N19" s="5"/>
@@ -953,14 +875,10 @@
       <c r="Q19" s="5"/>
       <c r="R19" s="5"/>
     </row>
-    <row r="20" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
-      <c r="B20" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" s="5">
-        <v>13</v>
-      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
@@ -968,7 +886,10 @@
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
+      <c r="K20" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="L20" s="5"/>
       <c r="M20" s="5"/>
       <c r="N20" s="5"/>
@@ -977,14 +898,10 @@
       <c r="Q20" s="5"/>
       <c r="R20" s="5"/>
     </row>
-    <row r="21" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
-      <c r="B21" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" s="5">
-        <v>14</v>
-      </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
@@ -992,7 +909,10 @@
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
+      <c r="K21" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="L21" s="5"/>
       <c r="M21" s="5"/>
       <c r="N21" s="5"/>
@@ -1001,14 +921,10 @@
       <c r="Q21" s="5"/>
       <c r="R21" s="5"/>
     </row>
-    <row r="22" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
-      <c r="B22" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C22" s="5">
-        <v>15</v>
-      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
@@ -1016,7 +932,10 @@
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
+      <c r="K22" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="L22" s="5"/>
       <c r="M22" s="5"/>
       <c r="N22" s="5"/>
@@ -1025,14 +944,10 @@
       <c r="Q22" s="5"/>
       <c r="R22" s="5"/>
     </row>
-    <row r="23" spans="1:18" ht="75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
-      <c r="B23" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C23" s="5">
-        <v>16</v>
-      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
@@ -1040,7 +955,10 @@
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
+      <c r="K23" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="L23" s="5"/>
       <c r="M23" s="5"/>
       <c r="N23" s="5"/>
@@ -1049,14 +967,10 @@
       <c r="Q23" s="5"/>
       <c r="R23" s="5"/>
     </row>
-    <row r="24" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
-      <c r="B24" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" s="5">
-        <v>17</v>
-      </c>
+      <c r="B24" s="4"/>
+      <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
@@ -1064,7 +978,10 @@
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
+      <c r="K24" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="L24" s="5"/>
       <c r="M24" s="5"/>
       <c r="N24" s="5"/>
@@ -1075,12 +992,8 @@
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
-      <c r="B25" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C25" s="5">
-        <v>18</v>
-      </c>
+      <c r="B25" s="4"/>
+      <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
@@ -1088,7 +1001,10 @@
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
-      <c r="K25" s="5"/>
+      <c r="K25" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="L25" s="5"/>
       <c r="M25" s="5"/>
       <c r="N25" s="5"/>
@@ -1099,12 +1015,8 @@
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
-      <c r="B26" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C26" s="5">
-        <v>19</v>
-      </c>
+      <c r="B26" s="4"/>
+      <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
@@ -1112,7 +1024,10 @@
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
-      <c r="K26" s="5"/>
+      <c r="K26" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="L26" s="5"/>
       <c r="M26" s="5"/>
       <c r="N26" s="5"/>
@@ -1123,12 +1038,8 @@
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
-      <c r="B27" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C27" s="5">
-        <v>20</v>
-      </c>
+      <c r="B27" s="4"/>
+      <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
@@ -1136,7 +1047,10 @@
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
-      <c r="K27" s="5"/>
+      <c r="K27" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="L27" s="5"/>
       <c r="M27" s="5"/>
       <c r="N27" s="5"/>
@@ -1145,14 +1059,10 @@
       <c r="Q27" s="5"/>
       <c r="R27" s="5"/>
     </row>
-    <row r="28" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
-      <c r="B28" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C28" s="5">
-        <v>21</v>
-      </c>
+      <c r="B28" s="4"/>
+      <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
@@ -1160,7 +1070,10 @@
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
-      <c r="K28" s="5"/>
+      <c r="K28" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="L28" s="5"/>
       <c r="M28" s="5"/>
       <c r="N28" s="5"/>
@@ -1169,14 +1082,10 @@
       <c r="Q28" s="5"/>
       <c r="R28" s="5"/>
     </row>
-    <row r="29" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
-      <c r="B29" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C29" s="5">
-        <v>22</v>
-      </c>
+      <c r="B29" s="4"/>
+      <c r="C29" s="5"/>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
@@ -1184,7 +1093,10 @@
       <c r="H29" s="6"/>
       <c r="I29" s="6"/>
       <c r="J29" s="6"/>
-      <c r="K29" s="6"/>
+      <c r="K29" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="L29" s="6"/>
       <c r="M29" s="6"/>
       <c r="N29" s="6"/>
@@ -1192,6 +1104,468 @@
       <c r="P29" s="6"/>
       <c r="Q29" s="6"/>
       <c r="R29" s="6"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="K30" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="K31" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="K32" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K33" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K34" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K35" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K36" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K37" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K38" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K39" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K40" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K41" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K42" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K43" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K44" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K45" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K46" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K47" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K48" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K49" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K50" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K51" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K52" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K53" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K54" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K55" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K56" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K57" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K58" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K59" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K60" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K61" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K62" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K63" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K64" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K65" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K66" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K67" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K68" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K69" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K70" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K71" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K72" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K73" s="5">
+        <f t="shared" ref="K73:K106" si="1">SUM(L73+M73+N73+O73+P73+Q73)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K74" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K75" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K76" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K77" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K78" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K79" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K80" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K81" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K82" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K83" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K84" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K85" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K86" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K87" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K88" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K89" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K90" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K91" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K92" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K93" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K94" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K95" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K96" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K97" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K98" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K99" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K100" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K101" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K102" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K103" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K104" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K105" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K106" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>